<commit_message>
Continuing analysis, problem with MrBIG efficiency
</commit_message>
<xml_diff>
--- a/divers/analysis.xlsx
+++ b/divers/analysis.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="distancescells" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="time_alignement" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="efficiency_monster" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="efficiency_monster_2" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="eff_mrbig" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="eff_beta" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="Pn" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="effge" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="eff_mrbig" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="eff_beta" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Pn" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="effge" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t xml:space="preserve">RUN29</t>
   </si>
@@ -530,19 +529,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+                <a:uFillTx/>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-                <a:ea typeface="DejaVu Sans"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:rPr>
@@ -590,10 +587,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFillTx/>
                     <a:latin typeface="Aptos Narrow"/>
                     <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
@@ -608,6 +606,13 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="38160">
+                  <a:noFill/>
+                </a:ln>
+              </c:spPr>
+            </c:leaderLines>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -742,11 +747,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="40871499"/>
-        <c:axId val="99902421"/>
+        <c:axId val="91564047"/>
+        <c:axId val="23782208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40871499"/>
+        <c:axId val="91564047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -779,22 +784,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99902421"/>
+        <c:crossAx val="23782208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99902421"/>
+        <c:axId val="23782208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,17 +833,18 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40871499"/>
+        <c:crossAx val="91564047"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -877,19 +884,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+                <a:uFillTx/>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-                <a:ea typeface="DejaVu Sans"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:rPr>
@@ -937,10 +942,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFillTx/>
                     <a:latin typeface="Aptos Narrow"/>
                     <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
@@ -955,580 +961,13 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>efficiency_monster!$J$13:$J$36</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="24"/>
-                  <c:pt idx="0">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.000226216924525648</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.000262827868101584</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.000258742738743185</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.000243486272091131</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0.000234322673473038</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0.000215839781559414</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.000208404122440775</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0.000200028079466069</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0.000197696651071629</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>0.000178493239788128</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>0.000173950176506118</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>0.000167653681062942</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0.000172017399496379</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0.000165150969022132</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>0.000155243092438848</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>0.000155666463177798</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>0.000144006344929081</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>0.000155487083974515</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>0.000147903230898418</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>0.000146712969051765</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>0.000142625711513344</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>0.00013475019109732</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>0.000146972229959489</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>efficiency_monster!$J$13:$J$36</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="24"/>
-                  <c:pt idx="0">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.000226216924525648</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.000262827868101584</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.000258742738743185</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.000243486272091131</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0.000234322673473038</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0.000215839781559414</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.000208404122440775</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0.000200028079466069</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0.000197696651071629</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>0.000178493239788128</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>0.000173950176506118</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>0.000167653681062942</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0.000172017399496379</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0.000165150969022132</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>0.000155243092438848</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>0.000155666463177798</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>0.000144006344929081</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>0.000155487083974515</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>0.000147903230898418</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>0.000146712969051765</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>0.000142625711513344</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>0.00013475019109732</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>0.000146972229959489</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:ln w="9360">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
-            <c:noEndCap val="0"/>
-            <c:val val="0"/>
-            <c:spPr>
-              <a:ln w="9360">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>efficiency_monster!$A$13:$A$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.4</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.6</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>4.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>efficiency_monster!$G$13:$G$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0250922123439437</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0291630505035158</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.028709465687776</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0270134998272188</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0259935632441897</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.023937282381879</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0231079101548389</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0221733164778677</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0219096481889452</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0197706594104667</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.0192595058984358</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.0185528845653561</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.0190295882026091</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.0182571198016345</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.0171457816831472</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0171804077406688</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0158708059037313</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.01713032633102</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0162692855035083</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0161159805789448</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0156378379163876</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0147354757929713</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0160620809783463</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="42987597"/>
-        <c:axId val="72188041"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="42987597"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-                <a:ea typeface="DejaVu Sans"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="72188041"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="72188041"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-                <a:ea typeface="DejaVu Sans"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="42987597"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-                <a:ea typeface="DejaVu Sans"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-                <a:ea typeface="DejaVu Sans"/>
-              </a:rPr>
-              <a:t>Chart Title</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="156082"/>
-            </a:solidFill>
-            <a:ln w="25560">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="156082"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Aptos Narrow"/>
-                    <a:ea typeface="DejaVu Sans"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="25560">
+                  <a:noFill/>
+                </a:ln>
+              </c:spPr>
+            </c:leaderLines>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1728,7 +1167,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>efficiency_monster_2!$A$13:$A$36</c:f>
+              <c:f>efficiency_monster!$A$13:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1809,7 +1248,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>efficiency_monster_2!$G$13:$G$36</c:f>
+              <c:f>efficiency_monster!$G$13:$G$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1890,11 +1329,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="23212197"/>
-        <c:axId val="77440590"/>
+        <c:axId val="6002628"/>
+        <c:axId val="27295874"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="23212197"/>
+        <c:axId val="6002628"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1927,22 +1366,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77440590"/>
+        <c:crossAx val="27295874"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77440590"/>
+        <c:axId val="27295874"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,17 +1415,18 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23212197"/>
+        <c:crossAx val="6002628"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2013,7 +1454,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2025,19 +1466,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+                <a:uFillTx/>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-                <a:ea typeface="DejaVu Sans"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:rPr>
@@ -2085,10 +1524,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFillTx/>
                     <a:latin typeface="Aptos Narrow"/>
                     <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
@@ -2103,6 +1543,13 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="25560">
+                  <a:noFill/>
+                </a:ln>
+              </c:spPr>
+            </c:leaderLines>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -2181,11 +1628,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="45599742"/>
-        <c:axId val="89548956"/>
+        <c:axId val="33712220"/>
+        <c:axId val="83337722"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45599742"/>
+        <c:axId val="33712220"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2218,22 +1665,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89548956"/>
+        <c:crossAx val="83337722"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89548956"/>
+        <c:axId val="83337722"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2266,17 +1714,18 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45599742"/>
+        <c:crossAx val="33712220"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2304,7 +1753,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2316,19 +1765,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+                <a:uFillTx/>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1400" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-                <a:ea typeface="DejaVu Sans"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:rPr>
@@ -2376,10 +1823,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFillTx/>
                     <a:latin typeface="Aptos Narrow"/>
                     <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
@@ -2394,6 +1842,13 @@
             <c:showPercent val="0"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="25560">
+                  <a:noFill/>
+                </a:ln>
+              </c:spPr>
+            </c:leaderLines>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -2472,11 +1927,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="49603387"/>
-        <c:axId val="74250932"/>
+        <c:axId val="79936384"/>
+        <c:axId val="5371632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49603387"/>
+        <c:axId val="79936384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2509,22 +1964,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74250932"/>
+        <c:crossAx val="5371632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74250932"/>
+        <c:axId val="5371632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2557,17 +2013,18 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
+                <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
                 <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49603387"/>
+        <c:crossAx val="79936384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2592,10 +2049,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr b="0" sz="900" strike="noStrike" u="none">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
+              <a:uFillTx/>
               <a:latin typeface="Aptos Narrow"/>
               <a:ea typeface="DejaVu Sans"/>
             </a:defRPr>
@@ -2631,18 +2089,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>177120</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:colOff>176760</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Graphique 3"/>
+        <xdr:cNvPr id="1" name="Graphique 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4699080" y="3942720"/>
-        <a:ext cx="17814240" cy="7741440"/>
+        <a:ext cx="17813880" cy="7741080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2668,16 +2126,16 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>31680</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>88200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Graphique 1"/>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13330080" y="3387960"/>
-        <a:ext cx="7377840" cy="4192200"/>
+        <a:off x="14418720" y="3387960"/>
+        <a:ext cx="7377480" cy="4191840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2694,41 +2152,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>99360</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>31680</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="13330080" y="3387960"/>
-        <a:ext cx="7377840" cy="4192200"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>108000</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -2736,9 +2159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>63000</xdr:colOff>
+      <xdr:colOff>62640</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2747,7 +2170,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="17744400" y="781560"/>
-        <a:ext cx="13782240" cy="7120080"/>
+        <a:ext cx="13781880" cy="7119720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2766,9 +2189,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>126360</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:colOff>126000</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2777,7 +2200,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5794560" y="7491600"/>
-        <a:ext cx="9812520" cy="5526720"/>
+        <a:ext cx="9812160" cy="5526360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2901,13 +2324,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -3104,6 +2527,26 @@
         <v>158</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3127,7 +2570,7 @@
       <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3593,13 +3036,14 @@
   </sheetPr>
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.87"/>
   </cols>
@@ -4974,1372 +4418,572 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N34" activeCellId="0" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>7260</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>37000</v>
-      </c>
-      <c r="N1" s="5"/>
-    </row>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>83412720</v>
-      </c>
-      <c r="P2" s="5"/>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>7300</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="L3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>40000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>95558400</v>
-      </c>
-      <c r="L4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="C4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>783</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="7" t="n">
+        <f aca="false">M3*EXP((-LN(2)/J10)*J7)</f>
+        <v>34840.3426838857</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
+      <c r="C5" s="6" t="n">
+        <v>661.6</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>56809.9</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>1292.09</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>591</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>821</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="7" t="n">
+        <f aca="false">M3*EXP((-LN(2)/J11)*J8)</f>
+        <v>18217.9426291197</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
+      <c r="C6" s="6" t="n">
+        <v>1173.228</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="I6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>2961</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>1011</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <f aca="false">M2*EXP((-LN(2)/J12)*J9)</f>
+        <v>6057.14624857478</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
+      <c r="C7" s="6" t="n">
+        <v>1332.492</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="I7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>188611200</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <f aca="false">H1*EXP((-LN(2)/H2)*B4)</f>
-        <v>16723.9521895749</v>
+      <c r="C8" s="6"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+      <c r="I8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>188611200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <f aca="false">B8*E1*3.7*0.0309</f>
-        <v>13881479.0348355</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="I9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>114994800</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="I10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>946647648</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="4"/>
+      <c r="I11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="7" t="n">
+        <v>166230000</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B12" s="4"/>
       <c r="I12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>427080000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <f aca="false">$B$9*B13</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <f aca="false">0.3*C13</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <f aca="false">SQRT(E13)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <f aca="false">SQRT(H13+I13)</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="n">
-        <f aca="false">0.05*G13</f>
-        <v>0</v>
-      </c>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="B14" s="4" t="n">
-        <v>0.30996667</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <f aca="false">$B$9*B14</f>
-        <v>4302795.83110279</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <f aca="false">0.3*C14</f>
-        <v>1290838.74933084</v>
+        <v>661.6</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>5631.31</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>3239</v>
-      </c>
-      <c r="F14" s="1" t="n">
-        <f aca="false">SQRT(E14)</f>
-        <v>56.9122131005288</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <f aca="false">E14/C14/0.03</f>
-        <v>0.0250922123439437</v>
-      </c>
-      <c r="H14" s="1" t="n">
-        <f aca="false">(F14/C14)^2</f>
-        <v>1.74948196444027E-010</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <f aca="false">(E14*D14/(C14^2))^2</f>
-        <v>5.09991487453982E-008</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <f aca="false">SQRT(H14+I14)</f>
-        <v>0.000226216924525647</v>
-      </c>
-      <c r="K14" s="1" t="n">
-        <f aca="false">0.1*G14</f>
-        <v>0.00250922123439437</v>
+        <v>7.39313</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="B15" s="4" t="n">
-        <v>0.3329</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <f aca="false">$B$9*B15</f>
-        <v>4621144.37069675</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <f aca="false">0.3*C15</f>
-        <v>1386343.31120903</v>
+      <c r="D15" s="4" t="n">
+        <v>56809.9</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>4043</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <f aca="false">SQRT(E15)</f>
-        <v>63.5845893279181</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <f aca="false">E15/C15/0.03</f>
-        <v>0.0291630505035157</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <f aca="false">(F15/C15)^2</f>
-        <v>1.89323562503969E-010</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <f aca="false">(E15*D15/(C15^2))^2</f>
-        <v>6.88891646883192E-008</v>
-      </c>
-      <c r="J15" s="1" t="n">
-        <f aca="false">SQRT(H15+I15)</f>
-        <v>0.000262827868101583</v>
-      </c>
-      <c r="K15" s="1" t="n">
-        <f aca="false">0.1*G15</f>
-        <v>0.00291630505035157</v>
+        <v>1.4125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <f aca="false">A15+0.2</f>
-        <v>0.8</v>
-      </c>
-      <c r="B16" s="4" t="n">
-        <v>0.33556667</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <f aca="false">$B$9*B16</f>
-        <v>4658161.69439458</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <f aca="false">0.3*C16</f>
-        <v>1397448.50831837</v>
+      <c r="D16" s="4" t="n">
+        <v>1292.09</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>4012</v>
-      </c>
-      <c r="F16" s="1" t="n">
-        <f aca="false">SQRT(E16)</f>
-        <v>63.3403504884525</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <f aca="false">E16/C16/0.03</f>
-        <v>0.0287094656877759</v>
-      </c>
-      <c r="H16" s="1" t="n">
-        <f aca="false">(F16/C16)^2</f>
-        <v>1.84897826039338E-010</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <f aca="false">(E16*D16/(C16^2))^2</f>
-        <v>6.67629070262842E-008</v>
-      </c>
-      <c r="J16" s="1" t="n">
-        <f aca="false">SQRT(H16+I16)</f>
-        <v>0.000258742738743184</v>
-      </c>
-      <c r="K16" s="1" t="n">
-        <f aca="false">0.1*G16</f>
-        <v>0.00287094656877759</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
-        <f aca="false">A16+0.2</f>
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="n">
-        <v>0.3289</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <f aca="false">$B$9*B17</f>
-        <v>4565618.45455741</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <f aca="false">0.3*C17</f>
-        <v>1369685.53636722</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>3700</v>
-      </c>
-      <c r="F17" s="1" t="n">
-        <f aca="false">SQRT(E17)</f>
-        <v>60.8276253029822</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <f aca="false">E17/C17/0.03</f>
-        <v>0.0270134998272187</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <f aca="false">(F17/C17)^2</f>
-        <v>1.7750169070909E-010</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <f aca="false">(E17*D17/(C17^2))^2</f>
-        <v>5.91080630061269E-008</v>
-      </c>
-      <c r="J17" s="1" t="n">
-        <f aca="false">SQRT(H17+I17)</f>
-        <v>0.00024348627209113</v>
-      </c>
-      <c r="K17" s="1" t="n">
-        <f aca="false">0.1*G17</f>
-        <v>0.00270134998272188</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <f aca="false">A17+0.2</f>
-        <v>1.2</v>
-      </c>
-      <c r="B18" s="4" t="n">
-        <v>0.3152</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <f aca="false">$B$9*B18</f>
-        <v>4375442.19178016</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <f aca="false">0.3*C18</f>
-        <v>1312632.65753405</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>3412</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <f aca="false">SQRT(E18)</f>
-        <v>58.4123274660409</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <f aca="false">E18/C18/0.03</f>
-        <v>0.0259935632441896</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <f aca="false">(F18/C18)^2</f>
-        <v>1.78223563047103E-010</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <f aca="false">(E18*D18/(C18^2))^2</f>
-        <v>5.47288917405045E-008</v>
-      </c>
-      <c r="J18" s="1" t="n">
-        <f aca="false">SQRT(H18+I18)</f>
-        <v>0.000234322673473037</v>
-      </c>
-      <c r="K18" s="1" t="n">
-        <f aca="false">0.1*G18</f>
-        <v>0.00259935632441896</v>
-      </c>
-    </row>
+        <v>1.10159</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <f aca="false">A18+0.2</f>
-        <v>1.4</v>
-      </c>
-      <c r="B19" s="4" t="n">
-        <v>0.29673333</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <f aca="false">$B$9*B19</f>
-        <v>4119097.49933194</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <f aca="false">0.3*C19</f>
-        <v>1235729.24979958</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>2958</v>
-      </c>
-      <c r="F19" s="1" t="n">
-        <f aca="false">SQRT(E19)</f>
-        <v>54.3874985635486</v>
-      </c>
-      <c r="G19" s="1" t="n">
-        <f aca="false">E19/C19/0.03</f>
-        <v>0.0239372823818789</v>
-      </c>
-      <c r="H19" s="1" t="n">
-        <f aca="false">(F19/C19)^2</f>
-        <v>1.74338789400551E-010</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <f aca="false">(E19*D19/(C19^2))^2</f>
-        <v>4.64124725142148E-008</v>
-      </c>
-      <c r="J19" s="1" t="n">
-        <f aca="false">SQRT(H19+I19)</f>
-        <v>0.000215839781559413</v>
-      </c>
-      <c r="K19" s="1" t="n">
-        <f aca="false">0.1*G19</f>
-        <v>0.00239372823818789</v>
-      </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+        <v>1173.228</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>1274.01</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>1476.13</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
-        <f aca="false">A19+0.2</f>
-        <v>1.6</v>
-      </c>
-      <c r="B20" s="4" t="n">
-        <v>0.27704</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <f aca="false">$B$9*B20</f>
-        <v>3845724.95181084</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <f aca="false">0.3*C20</f>
-        <v>1153717.48554325</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>2666</v>
-      </c>
-      <c r="F20" s="1" t="n">
-        <f aca="false">SQRT(E20)</f>
-        <v>51.6333225737023</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <f aca="false">E20/C20/0.03</f>
-        <v>0.0231079101548388</v>
-      </c>
-      <c r="H20" s="1" t="n">
-        <f aca="false">(F20/C20)^2</f>
-        <v>1.80261800657049E-010</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <f aca="false">(E20*D20/(C20^2))^2</f>
-        <v>4.32520164496523E-008</v>
-      </c>
-      <c r="J20" s="1" t="n">
-        <f aca="false">SQRT(H20+I20)</f>
-        <v>0.000208404122440774</v>
-      </c>
-      <c r="K20" s="1" t="n">
-        <f aca="false">0.1*G20</f>
-        <v>0.00231079101548388</v>
-      </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="D20" s="4" t="n">
+        <v>101044</v>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v>104317</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <f aca="false">A20+0.2</f>
-        <v>1.8</v>
-      </c>
-      <c r="B21" s="4" t="n">
-        <v>0.25612</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <f aca="false">$B$9*B21</f>
-        <v>3555324.41040208</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <f aca="false">0.3*C21</f>
-        <v>1066597.32312062</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>2365</v>
-      </c>
-      <c r="F21" s="1" t="n">
-        <f aca="false">SQRT(E21)</f>
-        <v>48.6312656631513</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <f aca="false">E21/C21/0.03</f>
-        <v>0.0221733164778676</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <f aca="false">(F21/C21)^2</f>
-        <v>1.87099521042244E-010</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <f aca="false">(E21*D21/(C21^2))^2</f>
-        <v>3.98241330538416E-008</v>
-      </c>
-      <c r="J21" s="1" t="n">
-        <f aca="false">SQRT(H21+I21)</f>
-        <v>0.000200028079466069</v>
-      </c>
-      <c r="K21" s="1" t="n">
-        <f aca="false">0.1*G21</f>
-        <v>0.00221733164778676</v>
-      </c>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <f aca="false">A21+0.2</f>
-        <v>2</v>
-      </c>
-      <c r="B22" s="4" t="n">
-        <v>0.2352</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <f aca="false">$B$9*B22</f>
-        <v>3264923.86899332</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <f aca="false">0.3*C22</f>
-        <v>979477.160697996</v>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>2146</v>
-      </c>
-      <c r="F22" s="1" t="n">
-        <f aca="false">SQRT(E22)</f>
-        <v>46.3249392876019</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <f aca="false">E22/C22/0.03</f>
-        <v>0.0219096481889452</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <f aca="false">(F22/C22)^2</f>
-        <v>2.01318460105784E-010</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <f aca="false">(E22*D22/(C22^2))^2</f>
-        <v>3.88826473848312E-008</v>
-      </c>
-      <c r="J22" s="1" t="n">
-        <f aca="false">SQRT(H22+I22)</f>
-        <v>0.000197696651071628</v>
-      </c>
-      <c r="K22" s="1" t="n">
-        <f aca="false">0.1*G22</f>
-        <v>0.00219096481889452</v>
-      </c>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <f aca="false">A22+0.2</f>
-        <v>2.2</v>
-      </c>
-      <c r="B23" s="4" t="n">
-        <v>0.2151</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <f aca="false">$B$9*B23</f>
-        <v>2985906.14039313</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <f aca="false">0.3*C23</f>
-        <v>895771.842117938</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>1771</v>
-      </c>
-      <c r="F23" s="1" t="n">
-        <f aca="false">SQRT(E23)</f>
-        <v>42.0832508250016</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <f aca="false">E23/C23/0.03</f>
-        <v>0.0197706594104666</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <f aca="false">(F23/C23)^2</f>
-        <v>1.98639794563639E-010</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <f aca="false">(E23*D23/(C23^2))^2</f>
-        <v>3.16611968554983E-008</v>
-      </c>
-      <c r="J23" s="1" t="n">
-        <f aca="false">SQRT(H23+I23)</f>
-        <v>0.000178493239788128</v>
-      </c>
-      <c r="K23" s="1" t="n">
-        <f aca="false">0.1*G23</f>
-        <v>0.00197706594104666</v>
-      </c>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-    </row>
-    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <f aca="false">A23+0.2</f>
-        <v>2.4</v>
-      </c>
-      <c r="B24" s="4" t="n">
-        <v>0.195</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <f aca="false">$B$9*B24</f>
-        <v>2706888.41179293</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <f aca="false">0.3*C24</f>
-        <v>812066.52353788</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>1564</v>
-      </c>
-      <c r="F24" s="1" t="n">
-        <f aca="false">SQRT(E24)</f>
-        <v>39.5474398665704</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <f aca="false">E24/C24/0.03</f>
-        <v>0.0192595058984357</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <f aca="false">(F24/C24)^2</f>
-        <v>2.13449942907093E-010</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <f aca="false">(E24*D24/(C24^2))^2</f>
-        <v>3.00452139636024E-008</v>
-      </c>
-      <c r="J24" s="1" t="n">
-        <f aca="false">SQRT(H24+I24)</f>
-        <v>0.000173950176506118</v>
-      </c>
-      <c r="K24" s="1" t="n">
-        <f aca="false">0.1*G24</f>
-        <v>0.00192595058984357</v>
-      </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-    </row>
+      <c r="D21" s="4" t="n">
+        <v>1556.41</v>
+      </c>
+      <c r="E21" s="4" t="n">
+        <v>1516.92</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <f aca="false">A24+0.2</f>
-        <v>2.6</v>
-      </c>
-      <c r="B25" s="4" t="n">
-        <v>0.1768</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <f aca="false">$B$9*B25</f>
-        <v>2454245.49335893</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <f aca="false">0.3*C25</f>
-        <v>736273.648007678</v>
-      </c>
-      <c r="E25" s="1" t="n">
-        <v>1366</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <f aca="false">SQRT(E25)</f>
-        <v>36.9594372251527</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <f aca="false">E25/C25/0.03</f>
-        <v>0.018552884565356</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <f aca="false">(F25/C25)^2</f>
-        <v>2.26785192625097E-010</v>
-      </c>
-      <c r="I25" s="1" t="n">
-        <f aca="false">(E25*D25/(C25^2))^2</f>
-        <v>2.78809715813294E-008</v>
-      </c>
-      <c r="J25" s="1" t="n">
-        <f aca="false">SQRT(H25+I25)</f>
-        <v>0.000167653681062942</v>
-      </c>
-      <c r="K25" s="1" t="n">
-        <f aca="false">0.1*G25</f>
-        <v>0.0018552884565356</v>
-      </c>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="I25" s="3" t="n">
+        <v>121.78</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>9678.28</v>
+      </c>
+      <c r="K25" s="3" t="n">
+        <f aca="false">(SQRT(2*PI())*D32*D34)/20</f>
+        <v>456466.700538131</v>
+      </c>
+      <c r="L25" s="3" t="n">
+        <v>0.2858</v>
+      </c>
+      <c r="M25" s="3" t="n">
+        <f aca="false">M6*L25*J6</f>
+        <v>5125883.03001215</v>
+      </c>
+      <c r="N25" s="3" t="n">
+        <f aca="false">100*K25/M25</f>
+        <v>8.90513298617056</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <f aca="false">0.1*N25</f>
+        <v>0.890513298617056</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <f aca="false">A25+0.2</f>
-        <v>2.8</v>
-      </c>
-      <c r="B26" s="4" t="n">
-        <v>0.1595</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <f aca="false">$B$9*B26</f>
-        <v>2214095.90605627</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <f aca="false">0.3*C26</f>
-        <v>664228.771816881</v>
-      </c>
-      <c r="E26" s="1" t="n">
-        <v>1264</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <f aca="false">SQRT(E26)</f>
-        <v>35.5527776692624</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <f aca="false">E26/C26/0.03</f>
-        <v>0.019029588202609</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <f aca="false">(F26/C26)^2</f>
-        <v>2.57842329465814E-010</v>
-      </c>
-      <c r="I26" s="1" t="n">
-        <f aca="false">(E26*D26/(C26^2))^2</f>
-        <v>2.9332143400031E-008</v>
-      </c>
-      <c r="J26" s="1" t="n">
-        <f aca="false">SQRT(H26+I26)</f>
-        <v>0.000172017399496379</v>
-      </c>
-      <c r="K26" s="1" t="n">
-        <f aca="false">0.1*G26</f>
-        <v>0.0019029588202609</v>
+        <v>1332.492</v>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>1111.86</v>
+      </c>
+      <c r="E26" s="4" t="n">
+        <v>1345.27</v>
+      </c>
+      <c r="I26" s="3" t="n">
+        <v>244.7</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>20584.2</v>
+      </c>
+      <c r="K26" s="3" t="n">
+        <f aca="false">(SQRT(2*PI())*D36*D38)/20</f>
+        <v>82070.1527808844</v>
+      </c>
+      <c r="L26" s="3" t="n">
+        <v>0.0758</v>
+      </c>
+      <c r="M26" s="3" t="n">
+        <f aca="false">M6*L26*J6</f>
+        <v>1359488.92118587</v>
+      </c>
+      <c r="N26" s="3" t="n">
+        <f aca="false">100*K26/M26</f>
+        <v>6.03683866061192</v>
+      </c>
+      <c r="O26" s="1" t="n">
+        <f aca="false">0.1*N26</f>
+        <v>0.603683866061192</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <f aca="false">A26+0.2</f>
-        <v>3</v>
-      </c>
-      <c r="B27" s="4" t="n">
-        <v>0.1431</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <f aca="false">$B$9*B27</f>
-        <v>1986439.64988497</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <f aca="false">0.3*C27</f>
-        <v>595931.89496549</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>1088</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <f aca="false">SQRT(E27)</f>
-        <v>32.9848450049413</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <f aca="false">E27/C27/0.03</f>
-        <v>0.0182571198016345</v>
-      </c>
-      <c r="H27" s="1" t="n">
-        <f aca="false">(F27/C27)^2</f>
-        <v>2.75726269398998E-010</v>
-      </c>
-      <c r="I27" s="1" t="n">
-        <f aca="false">(E27*D27/(C27^2))^2</f>
-        <v>2.69991162995499E-008</v>
-      </c>
-      <c r="J27" s="1" t="n">
-        <f aca="false">SQRT(H27+I27)</f>
-        <v>0.000165150969022131</v>
-      </c>
-      <c r="K27" s="1" t="n">
-        <f aca="false">0.1*G27</f>
-        <v>0.00182571198016345</v>
+      <c r="D27" s="4" t="n">
+        <v>114648</v>
+      </c>
+      <c r="E27" s="4" t="n">
+        <v>118307</v>
+      </c>
+      <c r="I27" s="3" t="n">
+        <v>344.28</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>29361.1</v>
+      </c>
+      <c r="K27" s="3" t="n">
+        <f aca="false">(SQRT(2*PI())*D40*D42)/20</f>
+        <v>290788.643643557</v>
+      </c>
+      <c r="L27" s="3" t="n">
+        <v>0.265</v>
+      </c>
+      <c r="M27" s="3" t="n">
+        <f aca="false">M6*L27*J6</f>
+        <v>4752830.66113793</v>
+      </c>
+      <c r="N27" s="3" t="n">
+        <f aca="false">100*K27/M27</f>
+        <v>6.11822015922477</v>
+      </c>
+      <c r="O27" s="1" t="n">
+        <f aca="false">0.1*N27</f>
+        <v>0.611822015922477</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <f aca="false">A27+0.2</f>
-        <v>3.2</v>
-      </c>
-      <c r="B28" s="4" t="n">
-        <v>0.12856667</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <f aca="false">$B$9*B28</f>
-        <v>1784695.53418362</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <f aca="false">0.3*C28</f>
-        <v>535408.660255086</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>918</v>
-      </c>
-      <c r="F28" s="1" t="n">
-        <f aca="false">SQRT(E28)</f>
-        <v>30.2985148150862</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <f aca="false">E28/C28/0.03</f>
-        <v>0.0171457816831471</v>
-      </c>
-      <c r="H28" s="1" t="n">
-        <f aca="false">(F28/C28)^2</f>
-        <v>2.88213558358964E-010</v>
-      </c>
-      <c r="I28" s="1" t="n">
-        <f aca="false">(E28*D28/(C28^2))^2</f>
-        <v>2.38122041916176E-008</v>
-      </c>
-      <c r="J28" s="1" t="n">
-        <f aca="false">SQRT(H28+I28)</f>
-        <v>0.000155243092438848</v>
-      </c>
-      <c r="K28" s="1" t="n">
-        <f aca="false">0.1*G28</f>
-        <v>0.00171457816831471</v>
+      <c r="D28" s="4" t="n">
+        <v>1714.67</v>
+      </c>
+      <c r="E28" s="4" t="n">
+        <v>1750.4</v>
+      </c>
+      <c r="I28" s="3" t="n">
+        <v>661.6</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>56809.9</v>
+      </c>
+      <c r="K28" s="3" t="n">
+        <f aca="false">(SQRT(2*PI())*D14*D16)/20</f>
+        <v>911931.336355026</v>
+      </c>
+      <c r="L28" s="3" t="n">
+        <v>0.8501</v>
+      </c>
+      <c r="M28" s="3" t="n">
+        <f aca="false">M4*L28*J4</f>
+        <v>23190718.0720922</v>
+      </c>
+      <c r="N28" s="3" t="n">
+        <f aca="false">100*K28/M28</f>
+        <v>3.9323117702528</v>
+      </c>
+      <c r="O28" s="1" t="n">
+        <f aca="false">0.1*N28</f>
+        <v>0.39323117702528</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <f aca="false">A28+0.2</f>
-        <v>3.4</v>
-      </c>
-      <c r="B29" s="4" t="n">
-        <v>0.11475</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <f aca="false">$B$9*B29</f>
-        <v>1592899.71924738</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <f aca="false">0.3*C29</f>
-        <v>477869.915774214</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>821</v>
-      </c>
-      <c r="F29" s="1" t="n">
-        <f aca="false">SQRT(E29)</f>
-        <v>28.6530975637888</v>
-      </c>
-      <c r="G29" s="1" t="n">
-        <f aca="false">E29/C29/0.03</f>
-        <v>0.0171804077406687</v>
-      </c>
-      <c r="H29" s="1" t="n">
-        <f aca="false">(F29/C29)^2</f>
-        <v>3.23568537298497E-010</v>
-      </c>
-      <c r="I29" s="1" t="n">
-        <f aca="false">(E29*D29/(C29^2))^2</f>
-        <v>2.39084792209859E-008</v>
-      </c>
-      <c r="J29" s="1" t="n">
-        <f aca="false">SQRT(H29+I29)</f>
-        <v>0.000155666463177797</v>
-      </c>
-      <c r="K29" s="1" t="n">
-        <f aca="false">0.1*G29</f>
-        <v>0.00171804077406687</v>
+      <c r="I29" s="3" t="n">
+        <v>1173.228</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>101044</v>
+      </c>
+      <c r="K29" s="3" t="n">
+        <f aca="false">(SQRT(2*PI())*D19*D21)/20</f>
+        <v>248517.392303561</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <v>0.9985</v>
+      </c>
+      <c r="M29" s="3" t="n">
+        <f aca="false">L29*M5*J5</f>
+        <v>10750653.8876691</v>
+      </c>
+      <c r="N29" s="3" t="n">
+        <f aca="false">100*K29/M29</f>
+        <v>2.31164908572314</v>
+      </c>
+      <c r="O29" s="1" t="n">
+        <f aca="false">0.1*N29</f>
+        <v>0.231164908572314</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <f aca="false">A29+0.2</f>
-        <v>3.6</v>
-      </c>
-      <c r="B30" s="4" t="n">
-        <v>0.10228</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <f aca="false">$B$9*B30</f>
-        <v>1419797.67568298</v>
-      </c>
-      <c r="D30" s="1" t="n">
-        <f aca="false">0.3*C30</f>
-        <v>425939.302704894</v>
-      </c>
-      <c r="E30" s="1" t="n">
-        <v>676</v>
-      </c>
-      <c r="F30" s="1" t="n">
-        <f aca="false">SQRT(E30)</f>
-        <v>26</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <f aca="false">E30/C30/0.03</f>
-        <v>0.0158708059037312</v>
-      </c>
-      <c r="H30" s="1" t="n">
-        <f aca="false">(F30/C30)^2</f>
-        <v>3.35346497086567E-010</v>
-      </c>
       <c r="I30" s="1" t="n">
-        <f aca="false">(E30*D30/(C30^2))^2</f>
-        <v>2.04024808827468E-008</v>
-      </c>
-      <c r="J30" s="1" t="n">
-        <f aca="false">SQRT(H30+I30)</f>
-        <v>0.000144006344929081</v>
+        <v>1332.492</v>
+      </c>
+      <c r="J30" s="4" t="n">
+        <v>114648</v>
       </c>
       <c r="K30" s="1" t="n">
-        <f aca="false">0.1*G30</f>
-        <v>0.00158708059037312</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <f aca="false">A30+0.2</f>
-        <v>3.8</v>
-      </c>
-      <c r="B31" s="4" t="n">
-        <v>0.090975</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <f aca="false">$B$9*B31</f>
-        <v>1262867.55519416</v>
-      </c>
-      <c r="D31" s="1" t="n">
-        <f aca="false">0.3*C31</f>
-        <v>378860.266558249</v>
-      </c>
-      <c r="E31" s="1" t="n">
-        <v>649</v>
-      </c>
-      <c r="F31" s="1" t="n">
-        <f aca="false">SQRT(E31)</f>
-        <v>25.475478405714</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <f aca="false">E31/C31/0.03</f>
-        <v>0.0171303263310199</v>
-      </c>
-      <c r="H31" s="1" t="n">
-        <f aca="false">(F31/C31)^2</f>
-        <v>4.06938786111727E-010</v>
-      </c>
-      <c r="I31" s="1" t="n">
-        <f aca="false">(E31*D31/(C31^2))^2</f>
-        <v>2.3769294496786E-008</v>
-      </c>
-      <c r="J31" s="1" t="n">
-        <f aca="false">SQRT(H31+I31)</f>
-        <v>0.000155487083974514</v>
-      </c>
-      <c r="K31" s="1" t="n">
-        <f aca="false">0.1*G31</f>
-        <v>0.00171303263310199</v>
-      </c>
-    </row>
+        <f aca="false">(SQRT(2*PI())*D26*D28)/20</f>
+        <v>238940.954601456</v>
+      </c>
+      <c r="L30" s="1" t="n">
+        <v>0.9998</v>
+      </c>
+      <c r="M30" s="1" t="n">
+        <f aca="false">M5*L30*J5</f>
+        <v>10764650.732991</v>
+      </c>
+      <c r="N30" s="1" t="n">
+        <f aca="false">100*K30/M30</f>
+        <v>2.21968144186193</v>
+      </c>
+      <c r="O30" s="1" t="n">
+        <f aca="false">0.1*N30</f>
+        <v>0.221968144186193</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <f aca="false">A31+0.2</f>
-        <v>4</v>
-      </c>
-      <c r="B32" s="4" t="n">
-        <v>0.080735</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <f aca="false">$B$9*B32</f>
-        <v>1120721.20987745</v>
-      </c>
-      <c r="D32" s="1" t="n">
-        <f aca="false">0.3*C32</f>
-        <v>336216.362963234</v>
-      </c>
-      <c r="E32" s="1" t="n">
-        <v>547</v>
-      </c>
-      <c r="F32" s="1" t="n">
-        <f aca="false">SQRT(E32)</f>
-        <v>23.388031127053</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <f aca="false">E32/C32/0.03</f>
-        <v>0.0162692855035082</v>
-      </c>
-      <c r="H32" s="1" t="n">
-        <f aca="false">(F32/C32)^2</f>
-        <v>4.35503995823027E-010</v>
-      </c>
-      <c r="I32" s="1" t="n">
-        <f aca="false">(E32*D32/(C32^2))^2</f>
-        <v>2.14398617143676E-008</v>
-      </c>
-      <c r="J32" s="1" t="n">
-        <f aca="false">SQRT(H32+I32)</f>
-        <v>0.000147903230898418</v>
-      </c>
-      <c r="K32" s="1" t="n">
-        <f aca="false">0.1*G32</f>
-        <v>0.00162692855035082</v>
+        <v>121.78</v>
+      </c>
+      <c r="D32" s="10" t="n">
+        <v>4576.9</v>
+      </c>
+      <c r="E32" s="11" t="n">
+        <v>3508.5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <f aca="false">A32+0.2</f>
-        <v>4.2</v>
-      </c>
-      <c r="B33" s="4" t="n">
-        <v>0.07152</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <f aca="false">$B$9*B33</f>
-        <v>992803.380571438</v>
-      </c>
-      <c r="D33" s="1" t="n">
-        <f aca="false">0.3*C33</f>
-        <v>297841.014171432</v>
-      </c>
-      <c r="E33" s="1" t="n">
-        <v>480</v>
-      </c>
-      <c r="F33" s="1" t="n">
-        <f aca="false">SQRT(E33)</f>
-        <v>21.9089023002066</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <f aca="false">E33/C33/0.03</f>
-        <v>0.0161159805789448</v>
-      </c>
-      <c r="H33" s="1" t="n">
-        <f aca="false">(F33/C33)^2</f>
-        <v>4.86984056289234E-010</v>
-      </c>
-      <c r="I33" s="1" t="n">
-        <f aca="false">(E33*D33/(C33^2))^2</f>
-        <v>2.10377112316949E-008</v>
-      </c>
-      <c r="J33" s="1" t="n">
-        <f aca="false">SQRT(H33+I33)</f>
-        <v>0.000146712969051765</v>
-      </c>
-      <c r="K33" s="1" t="n">
-        <f aca="false">0.1*G33</f>
-        <v>0.00161159805789448</v>
+      <c r="D33" s="10" t="n">
+        <v>9678.28</v>
+      </c>
+      <c r="E33" s="11" t="n">
+        <v>10916.4</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <f aca="false">A33+0.2</f>
-        <v>4.4</v>
-      </c>
-      <c r="B34" s="4" t="n">
-        <v>0.063265</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <f aca="false">$B$9*B34</f>
-        <v>878211.771138871</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <f aca="false">0.3*C34</f>
-        <v>263463.531341661</v>
-      </c>
-      <c r="E34" s="1" t="n">
-        <v>412</v>
-      </c>
-      <c r="F34" s="1" t="n">
-        <f aca="false">SQRT(E34)</f>
-        <v>20.2977831301844</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <f aca="false">E34/C34/0.03</f>
-        <v>0.0156378379163876</v>
-      </c>
-      <c r="H34" s="1" t="n">
-        <f aca="false">(F34/C34)^2</f>
-        <v>5.34193634051671E-010</v>
-      </c>
-      <c r="I34" s="1" t="n">
-        <f aca="false">(E34*D34/(C34^2))^2</f>
-        <v>1.98078999506359E-008</v>
-      </c>
-      <c r="J34" s="1" t="n">
-        <f aca="false">SQRT(H34+I34)</f>
-        <v>0.000142625711513344</v>
-      </c>
-      <c r="K34" s="1" t="n">
-        <f aca="false">0.1*G34</f>
-        <v>0.00156378379163876</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <f aca="false">A34+0.2</f>
-        <v>4.6</v>
-      </c>
-      <c r="B35" s="4" t="n">
-        <v>0.055895</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <f aca="false">$B$9*B35</f>
-        <v>775905.270652133</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <f aca="false">0.3*C35</f>
-        <v>232771.58119564</v>
-      </c>
-      <c r="E35" s="1" t="n">
-        <v>343</v>
-      </c>
-      <c r="F35" s="1" t="n">
-        <f aca="false">SQRT(E35)</f>
-        <v>18.5202591774521</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <f aca="false">E35/C35/0.03</f>
-        <v>0.0147354757929713</v>
-      </c>
-      <c r="H35" s="1" t="n">
-        <f aca="false">(F35/C35)^2</f>
-        <v>5.6974000629947E-010</v>
-      </c>
-      <c r="I35" s="1" t="n">
-        <f aca="false">(E35*D35/(C35^2))^2</f>
-        <v>1.75878739944646E-008</v>
-      </c>
-      <c r="J35" s="1" t="n">
-        <f aca="false">SQRT(H35+I35)</f>
-        <v>0.000134750191097319</v>
-      </c>
-      <c r="K35" s="1" t="n">
-        <f aca="false">0.1*G35</f>
-        <v>0.00147354757929713</v>
-      </c>
-    </row>
+      <c r="D34" s="10" t="n">
+        <v>795.752</v>
+      </c>
+      <c r="E34" s="11" t="n">
+        <v>532.225</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <f aca="false">A35+0.2</f>
-        <v>4.8</v>
-      </c>
-      <c r="B36" s="4" t="n">
-        <v>0.049335</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <f aca="false">$B$9*B36</f>
-        <v>684842.768183612</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <f aca="false">0.3*C36</f>
-        <v>205452.830455084</v>
-      </c>
-      <c r="E36" s="1" t="n">
-        <v>330</v>
-      </c>
-      <c r="F36" s="1" t="n">
-        <f aca="false">SQRT(E36)</f>
-        <v>18.165902124585</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <f aca="false">E36/C36/0.03</f>
-        <v>0.0160620809783463</v>
-      </c>
-      <c r="H36" s="1" t="n">
-        <f aca="false">(F36/C36)^2</f>
-        <v>7.03610305513509E-010</v>
-      </c>
-      <c r="I36" s="1" t="n">
-        <f aca="false">(E36*D36/(C36^2))^2</f>
-        <v>2.08972260737512E-008</v>
-      </c>
-      <c r="J36" s="1" t="n">
-        <f aca="false">SQRT(H36+I36)</f>
-        <v>0.000146972229959488</v>
-      </c>
-      <c r="K36" s="1" t="n">
-        <f aca="false">0.1*G36</f>
-        <v>0.00160620809783463</v>
+        <v>244.7</v>
+      </c>
+      <c r="D36" s="10" t="n">
+        <v>706.317</v>
+      </c>
+      <c r="E36" s="11" t="n">
+        <v>458.275</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <f aca="false">A36+0.2</f>
-        <v>5</v>
-      </c>
-      <c r="B37" s="4"/>
+      <c r="D37" s="10" t="n">
+        <v>20584.2</v>
+      </c>
+      <c r="E37" s="11" t="n">
+        <v>22015.4</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <f aca="false">A37+0.2</f>
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <f aca="false">A38+0.2</f>
-        <v>5.4</v>
-      </c>
-    </row>
+      <c r="D38" s="10" t="n">
+        <v>927.098</v>
+      </c>
+      <c r="E38" s="11" t="n">
+        <v>658.115</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <f aca="false">A39+0.2</f>
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <f aca="false">A40+0.2</f>
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <f aca="false">A41+0.2</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <f aca="false">A42+0.2</f>
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <f aca="false">A43+0.2</f>
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <f aca="false">A44+0.2</f>
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <f aca="false">A45+0.2</f>
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <f aca="false">A46+0.2</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <f aca="false">A47+0.2</f>
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <f aca="false">A48+0.2</f>
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <f aca="false">A49+0.2</f>
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
-        <f aca="false">A50+0.2</f>
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
-        <f aca="false">A51+0.2</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
-        <f aca="false">A52+0.2</f>
-        <v>8.2</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
-        <f aca="false">A53+0.2</f>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
-        <f aca="false">A54+0.2</f>
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
-        <f aca="false">A55+0.2</f>
-        <v>8.8</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
-        <f aca="false">A56+0.2</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
-        <f aca="false">A57+0.2</f>
-        <v>9.2</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
-        <f aca="false">A58+0.2</f>
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
-        <f aca="false">A59+0.2</f>
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
-        <f aca="false">A60+0.2</f>
-        <v>9.8</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
-        <f aca="false">A61+0.2</f>
-        <v>10</v>
-      </c>
-    </row>
+        <v>344.28</v>
+      </c>
+      <c r="D40" s="10" t="n">
+        <v>2203.86</v>
+      </c>
+      <c r="E40" s="11" t="n">
+        <v>1438.28</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="10" t="n">
+        <v>29361.1</v>
+      </c>
+      <c r="E41" s="11" t="n">
+        <v>30934.1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="10" t="n">
+        <v>1052.77</v>
+      </c>
+      <c r="E42" s="11" t="n">
+        <v>778.821</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -6357,572 +5001,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O42"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N34" activeCellId="0" sqref="N34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.75"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>7300</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>783</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="7" t="n">
-        <f aca="false">M3*EXP((-LN(2)/J10)*J7)</f>
-        <v>34840.3426838857</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="6" t="n">
-        <v>661.6</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>56809.9</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>1292.09</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="I5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>591</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>821</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="7" t="n">
-        <f aca="false">M3*EXP((-LN(2)/J11)*J8)</f>
-        <v>18217.9426291197</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="6" t="n">
-        <v>1173.228</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-      <c r="I6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>2961</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>1011</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="7" t="n">
-        <f aca="false">M2*EXP((-LN(2)/J12)*J9)</f>
-        <v>6057.14624857478</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="6" t="n">
-        <v>1332.492</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-      <c r="I7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>188611200</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="6"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="I8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <v>188611200</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="6"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="I9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <v>114994800</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="8" t="n">
-        <v>50000</v>
-      </c>
-      <c r="D10" s="8" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="I10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="1" t="n">
-        <v>946647648</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="4"/>
-      <c r="I11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="7" t="n">
-        <v>166230000</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="4"/>
-      <c r="I12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="5" t="n">
-        <v>427080000</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>661.6</v>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>5631.31</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>7.39313</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="4" t="n">
-        <v>56809.9</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>1.4125</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="4" t="n">
-        <v>1292.09</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>1.10159</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>1173.228</v>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>1274.01</v>
-      </c>
-      <c r="E19" s="4" t="n">
-        <v>1476.13</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="4" t="n">
-        <v>101044</v>
-      </c>
-      <c r="E20" s="4" t="n">
-        <v>104317</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="4" t="n">
-        <v>1556.41</v>
-      </c>
-      <c r="E21" s="4" t="n">
-        <v>1516.92</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I25" s="3" t="n">
-        <v>121.78</v>
-      </c>
-      <c r="J25" s="2" t="n">
-        <v>9678.28</v>
-      </c>
-      <c r="K25" s="3" t="n">
-        <f aca="false">(SQRT(2*PI())*D32*D34)/20</f>
-        <v>456466.700538131</v>
-      </c>
-      <c r="L25" s="3" t="n">
-        <v>0.2858</v>
-      </c>
-      <c r="M25" s="3" t="n">
-        <f aca="false">M6*L25*J6</f>
-        <v>5125883.03001215</v>
-      </c>
-      <c r="N25" s="3" t="n">
-        <f aca="false">100*K25/M25</f>
-        <v>8.90513298617056</v>
-      </c>
-      <c r="O25" s="1" t="n">
-        <f aca="false">0.1*N25</f>
-        <v>0.890513298617056</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
-        <v>1332.492</v>
-      </c>
-      <c r="D26" s="4" t="n">
-        <v>1111.86</v>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>1345.27</v>
-      </c>
-      <c r="I26" s="3" t="n">
-        <v>244.7</v>
-      </c>
-      <c r="J26" s="2" t="n">
-        <v>20584.2</v>
-      </c>
-      <c r="K26" s="3" t="n">
-        <f aca="false">(SQRT(2*PI())*D36*D38)/20</f>
-        <v>82070.1527808844</v>
-      </c>
-      <c r="L26" s="3" t="n">
-        <v>0.0758</v>
-      </c>
-      <c r="M26" s="3" t="n">
-        <f aca="false">M6*L26*J6</f>
-        <v>1359488.92118587</v>
-      </c>
-      <c r="N26" s="3" t="n">
-        <f aca="false">100*K26/M26</f>
-        <v>6.03683866061192</v>
-      </c>
-      <c r="O26" s="1" t="n">
-        <f aca="false">0.1*N26</f>
-        <v>0.603683866061192</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="4" t="n">
-        <v>114648</v>
-      </c>
-      <c r="E27" s="4" t="n">
-        <v>118307</v>
-      </c>
-      <c r="I27" s="3" t="n">
-        <v>344.28</v>
-      </c>
-      <c r="J27" s="2" t="n">
-        <v>29361.1</v>
-      </c>
-      <c r="K27" s="3" t="n">
-        <f aca="false">(SQRT(2*PI())*D40*D42)/20</f>
-        <v>290788.643643557</v>
-      </c>
-      <c r="L27" s="3" t="n">
-        <v>0.265</v>
-      </c>
-      <c r="M27" s="3" t="n">
-        <f aca="false">M6*L27*J6</f>
-        <v>4752830.66113793</v>
-      </c>
-      <c r="N27" s="3" t="n">
-        <f aca="false">100*K27/M27</f>
-        <v>6.11822015922477</v>
-      </c>
-      <c r="O27" s="1" t="n">
-        <f aca="false">0.1*N27</f>
-        <v>0.611822015922477</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="4" t="n">
-        <v>1714.67</v>
-      </c>
-      <c r="E28" s="4" t="n">
-        <v>1750.4</v>
-      </c>
-      <c r="I28" s="3" t="n">
-        <v>661.6</v>
-      </c>
-      <c r="J28" s="2" t="n">
-        <v>56809.9</v>
-      </c>
-      <c r="K28" s="3" t="n">
-        <f aca="false">(SQRT(2*PI())*D14*D16)/20</f>
-        <v>911931.336355026</v>
-      </c>
-      <c r="L28" s="3" t="n">
-        <v>0.8501</v>
-      </c>
-      <c r="M28" s="3" t="n">
-        <f aca="false">M4*L28*J4</f>
-        <v>23190718.0720922</v>
-      </c>
-      <c r="N28" s="3" t="n">
-        <f aca="false">100*K28/M28</f>
-        <v>3.9323117702528</v>
-      </c>
-      <c r="O28" s="1" t="n">
-        <f aca="false">0.1*N28</f>
-        <v>0.39323117702528</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I29" s="3" t="n">
-        <v>1173.228</v>
-      </c>
-      <c r="J29" s="2" t="n">
-        <v>101044</v>
-      </c>
-      <c r="K29" s="3" t="n">
-        <f aca="false">(SQRT(2*PI())*D19*D21)/20</f>
-        <v>248517.392303561</v>
-      </c>
-      <c r="L29" s="3" t="n">
-        <v>0.9985</v>
-      </c>
-      <c r="M29" s="3" t="n">
-        <f aca="false">L29*M5*J5</f>
-        <v>10750653.8876691</v>
-      </c>
-      <c r="N29" s="3" t="n">
-        <f aca="false">100*K29/M29</f>
-        <v>2.31164908572314</v>
-      </c>
-      <c r="O29" s="1" t="n">
-        <f aca="false">0.1*N29</f>
-        <v>0.231164908572314</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I30" s="1" t="n">
-        <v>1332.492</v>
-      </c>
-      <c r="J30" s="4" t="n">
-        <v>114648</v>
-      </c>
-      <c r="K30" s="1" t="n">
-        <f aca="false">(SQRT(2*PI())*D26*D28)/20</f>
-        <v>238940.954601456</v>
-      </c>
-      <c r="L30" s="1" t="n">
-        <v>0.9998</v>
-      </c>
-      <c r="M30" s="1" t="n">
-        <f aca="false">M5*L30*J5</f>
-        <v>10764650.732991</v>
-      </c>
-      <c r="N30" s="1" t="n">
-        <f aca="false">100*K30/M30</f>
-        <v>2.21968144186193</v>
-      </c>
-      <c r="O30" s="1" t="n">
-        <f aca="false">0.1*N30</f>
-        <v>0.221968144186193</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>121.78</v>
-      </c>
-      <c r="D32" s="10" t="n">
-        <v>4576.9</v>
-      </c>
-      <c r="E32" s="11" t="n">
-        <v>3508.5</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="10" t="n">
-        <v>9678.28</v>
-      </c>
-      <c r="E33" s="11" t="n">
-        <v>10916.4</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="10" t="n">
-        <v>795.752</v>
-      </c>
-      <c r="E34" s="11" t="n">
-        <v>532.225</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>244.7</v>
-      </c>
-      <c r="D36" s="10" t="n">
-        <v>706.317</v>
-      </c>
-      <c r="E36" s="11" t="n">
-        <v>458.275</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="10" t="n">
-        <v>20584.2</v>
-      </c>
-      <c r="E37" s="11" t="n">
-        <v>22015.4</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="10" t="n">
-        <v>927.098</v>
-      </c>
-      <c r="E38" s="11" t="n">
-        <v>658.115</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>344.28</v>
-      </c>
-      <c r="D40" s="10" t="n">
-        <v>2203.86</v>
-      </c>
-      <c r="E40" s="11" t="n">
-        <v>1438.28</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="10" t="n">
-        <v>29361.1</v>
-      </c>
-      <c r="E41" s="11" t="n">
-        <v>30934.1</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="10" t="n">
-        <v>1052.77</v>
-      </c>
-      <c r="E42" s="11" t="n">
-        <v>778.821</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7144,18 +5229,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:K39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="11.87"/>
@@ -7361,18 +5446,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:S87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J84" activeCellId="0" sqref="J84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I54" activeCellId="0" sqref="I54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.63"/>

</xml_diff>